<commit_message>
doc_Dokumentation ergänzt und verbessert doc_Container Sprints Kap.7 und andere ergänzt und verbessert
</commit_message>
<xml_diff>
--- a/doc/projectFiles/Zeiterfassung.xlsx
+++ b/doc/projectFiles/Zeiterfassung.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22221"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView visibility="hidden" xWindow="240" yWindow="40" windowWidth="20120" windowHeight="8000"/>
   </bookViews>
   <sheets>
     <sheet name="März" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,12 @@
     <sheet name="Juni" sheetId="5" r:id="rId4"/>
     <sheet name="Auswertung" sheetId="8" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -120,8 +124,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,25 +152,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -174,31 +178,31 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,7 +654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -658,14 +662,14 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="10"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="10"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -698,7 +702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1">
+    <row r="2" spans="1:13" ht="15" thickBot="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -939,7 +943,7 @@
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="11" spans="1:13" ht="15" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>25</v>
@@ -965,7 +969,7 @@
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="15.75" collapsed="1" thickBot="1">
+    <row r="12" spans="1:13" ht="15" collapsed="1" thickBot="1">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -7471,7 +7475,7 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="H258" s="9">
-        <f t="shared" ref="H258:H321" si="82">G258-F258</f>
+        <f t="shared" ref="H258:H302" si="82">G258-F258</f>
         <v>0.8571428571428571</v>
       </c>
       <c r="I258" s="5">
@@ -8809,9 +8813,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8824,12 +8828,17 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8837,13 +8846,13 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="10"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="10"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -15640,7 +15649,7 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="H258" s="8">
-        <f t="shared" ref="H258:H321" si="44">G258-F258</f>
+        <f t="shared" ref="H258:H301" si="44">G258-F258</f>
         <v>0.8571428571428571</v>
       </c>
       <c r="I258" s="1">
@@ -16800,9 +16809,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -16810,12 +16819,17 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16823,13 +16837,13 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -23629,7 +23643,7 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="H258" s="8">
-        <f t="shared" ref="H258:H321" si="42">G258-F258</f>
+        <f t="shared" ref="H258:H311" si="42">G258-F258</f>
         <v>0.8571428571428571</v>
       </c>
       <c r="I258" s="1">
@@ -24972,9 +24986,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -24997,9 +25011,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -25007,12 +25021,17 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25020,13 +25039,13 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -31826,7 +31845,7 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="H258" s="8">
-        <f t="shared" ref="H258:H321" si="37">G258-F258</f>
+        <f t="shared" ref="H258:H301" si="37">G258-F258</f>
         <v>0.8571428571428571</v>
       </c>
       <c r="I258" s="1">
@@ -32994,9 +33013,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -33009,9 +33028,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -33019,21 +33038,26 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:3">
@@ -33043,5 +33067,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>